<commit_message>
Updated main.py codes Added lines of code to generate 2 additional workbooks
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="155">
   <si>
     <t xml:space="preserve">PN</t>
   </si>
@@ -40,229 +40,451 @@
     <t xml:space="preserve">154581-04</t>
   </si>
   <si>
+    <t xml:space="preserve">IPC, RIGHT, BLK 20, CX-3 2.2.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">SN</t>
   </si>
   <si>
     <t xml:space="preserve">154580-04</t>
   </si>
   <si>
+    <t xml:space="preserve">IPC, LEFT, BLK 20, CX-3 2.2.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">151043-06</t>
   </si>
   <si>
+    <t xml:space="preserve">ASSY, COMMS, DIVERSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">150931-01</t>
   </si>
   <si>
+    <t xml:space="preserve">HARNESS AS, BLUE, CAM AFT - MK30-CX-3</t>
+  </si>
+  <si>
     <t xml:space="preserve">150932-01</t>
   </si>
   <si>
+    <t xml:space="preserve">HARNESS AS, PINK, AVIO RIGHT - MK30-CX-3</t>
+  </si>
+  <si>
     <t xml:space="preserve">150933-01</t>
   </si>
   <si>
+    <t xml:space="preserve">HARNESS AS, GREEN, CAM FWD - MK30-CX-3</t>
+  </si>
+  <si>
     <t xml:space="preserve">150930-02</t>
   </si>
   <si>
+    <t xml:space="preserve">HARNESS AS, BROWN, AVIO LEFT - MK30-CX-3</t>
+  </si>
+  <si>
     <t xml:space="preserve">151027-01</t>
   </si>
   <si>
+    <t xml:space="preserve">ASSY, AIR DATA SENSOR</t>
+  </si>
+  <si>
     <t xml:space="preserve">160272-02</t>
   </si>
   <si>
+    <t xml:space="preserve">PROPELLER ASSY, MK30, OFF-CENTER, CW</t>
+  </si>
+  <si>
     <t xml:space="preserve">160275-02</t>
   </si>
   <si>
+    <t xml:space="preserve">PROPELLER ASSY, MK30, CENTER, CCW</t>
+  </si>
+  <si>
     <t xml:space="preserve">160273-02</t>
   </si>
   <si>
+    <t xml:space="preserve">PROPELLER ASSY, MK30, OFF-CENTER, CCW</t>
+  </si>
+  <si>
     <t xml:space="preserve">160274-02</t>
   </si>
   <si>
+    <t xml:space="preserve">PROPELLER ASSY, MK30, CENTER, CW</t>
+  </si>
+  <si>
     <t xml:space="preserve">147702-05</t>
   </si>
   <si>
+    <t xml:space="preserve">ASSY, PDM, CX-3 IAW</t>
+  </si>
+  <si>
     <t xml:space="preserve">147080-03</t>
   </si>
   <si>
+    <t xml:space="preserve">RANGEFINDER, MK30</t>
+  </si>
+  <si>
     <t xml:space="preserve">153933-01</t>
   </si>
   <si>
+    <t xml:space="preserve">ASSY, SENSOR LRU, PUMA</t>
+  </si>
+  <si>
     <t xml:space="preserve">154045-01</t>
   </si>
   <si>
+    <t xml:space="preserve">ASSY, SENSOR LRU, VISTA</t>
+  </si>
+  <si>
     <t xml:space="preserve">156394-02</t>
   </si>
   <si>
+    <t xml:space="preserve">CX-3 LIGHTING, ASSY, RH, BLK20</t>
+  </si>
+  <si>
     <t xml:space="preserve">156393-02</t>
   </si>
   <si>
+    <t xml:space="preserve">CX-3 LIGHTING, ASSY, LH, BLK20</t>
+  </si>
+  <si>
     <t xml:space="preserve">150405-01</t>
   </si>
   <si>
+    <t xml:space="preserve">STRUT ASSY, UPR, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">147712-03</t>
   </si>
   <si>
+    <t xml:space="preserve">LRU, MOTOR, CX-3, IAW</t>
+  </si>
+  <si>
     <t xml:space="preserve">150416-01</t>
   </si>
   <si>
+    <t xml:space="preserve">STRUT ASSY, UPR, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150422-01</t>
   </si>
   <si>
+    <t xml:space="preserve">STRUT ASSY, MID, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150434-01</t>
   </si>
   <si>
+    <t xml:space="preserve">STRUT ASSY, MID, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150446-01</t>
   </si>
   <si>
+    <t xml:space="preserve">STRUT ASSY, LWR, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150462-01</t>
   </si>
   <si>
+    <t xml:space="preserve">STRUT ASSY, LWR, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">156976-02</t>
   </si>
   <si>
+    <t xml:space="preserve">ASSY, FRIDGE, BLK20</t>
+  </si>
+  <si>
     <t xml:space="preserve">147838-10</t>
   </si>
   <si>
+    <t xml:space="preserve">CELLULAR COMMS, MK30</t>
+  </si>
+  <si>
     <t xml:space="preserve">159860-01</t>
   </si>
   <si>
+    <t xml:space="preserve">INTEGRATED FAIRING ASSY, UPPER</t>
+  </si>
+  <si>
     <t xml:space="preserve">152350-02</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, BOTTOM ASSY</t>
+  </si>
+  <si>
     <t xml:space="preserve">LOT</t>
   </si>
   <si>
     <t xml:space="preserve">150308-02</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, BATTERY, RH, ASSY</t>
+  </si>
+  <si>
     <t xml:space="preserve">150298-02</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, BATTERY, LH, ASSY</t>
+  </si>
+  <si>
     <t xml:space="preserve">152347-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, SOB ASSY, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">152349-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, SOB ASSY, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">152348-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, AFT ASSY, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">152346-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, AFT ASSY, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">152352-02</t>
   </si>
   <si>
+    <t xml:space="preserve">NOSE CONE ASSY</t>
+  </si>
+  <si>
     <t xml:space="preserve">150483-02</t>
   </si>
   <si>
+    <t xml:space="preserve">WING ASSY, UPR</t>
+  </si>
+  <si>
     <t xml:space="preserve">150479-01</t>
   </si>
   <si>
+    <t xml:space="preserve">WINGLET ASSY, UPR, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150475-01</t>
   </si>
   <si>
+    <t xml:space="preserve">WINGLET ASSY, UPR, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150503-02</t>
   </si>
   <si>
+    <t xml:space="preserve">WING ASSY, LWR</t>
+  </si>
+  <si>
     <t xml:space="preserve">150490-01</t>
   </si>
   <si>
+    <t xml:space="preserve">WINGLET ASSY, LWR, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150494-01</t>
   </si>
   <si>
+    <t xml:space="preserve">WINGLET ASSY, LWR, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150500-02</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING ASSY, WING, LOWER, RH, UPPER SIDE</t>
+  </si>
+  <si>
     <t xml:space="preserve">150509-02</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, WING, LOWER, LH, LOWER SIDE</t>
+  </si>
+  <si>
     <t xml:space="preserve">150510-02</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, WING, LOWER, RH, LOWER SIDE</t>
+  </si>
+  <si>
     <t xml:space="preserve">150498-02</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING ASSY, WING, LOWER, LH, UPPER SIDE</t>
+  </si>
+  <si>
     <t xml:space="preserve">151008-01</t>
   </si>
   <si>
+    <t xml:space="preserve">SPINNER, MK30, OFF-CENTER</t>
+  </si>
+  <si>
     <t xml:space="preserve">151009-01</t>
   </si>
   <si>
+    <t xml:space="preserve">SPINNER, MK30, CENTER</t>
+  </si>
+  <si>
     <t xml:space="preserve">148234-01</t>
   </si>
   <si>
+    <t xml:space="preserve">LATCH, PUSH-PULL, 0.37" BOLT PROJECTION</t>
+  </si>
+  <si>
     <t xml:space="preserve">156231-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, MOTOR MOUNT, UPR, INBD, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">156234-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, MOTOR MOUNT, UPR, INBD, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">156232-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING ASSY, MOTOR MOUNT, UPR, OUTBD, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">156235-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING ASSY, MOTOR MOUNT, UPR, OUTBD, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150515-02</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING ASSY, WING, UPPER, OUTBD, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150524-02</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, WING, UPPER, INBD, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150525-02</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, WING, UPPER, INBD, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150517-02</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING ASSY, WING, UPPER, OUTBD, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">156228-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING ASSY, MOTOR MOUNT, MID, UPR, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">156227-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, MOTOR MOUNT, MID, LWR, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">156224-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING ASSY, MOTOR MOUNT, MID, UPR, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">156223-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, MOTOR MOUNT, MID, LWR, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">156359-01</t>
   </si>
   <si>
+    <t xml:space="preserve">LANDING GEAR, ASSY, WHEEL, SECONDARY</t>
+  </si>
+  <si>
     <t xml:space="preserve">156219-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, MOTOR MOUNT, LWR, OUTBD, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">156220-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING ASSY, MOTOR MOUNT, LWR, INBD, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">156238-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING ASSY, MOTOR MOUNT, LWR, INBD, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">156217-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIRING, MOTOR MOUNT, LWR, OUTBD, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150364-02</t>
   </si>
   <si>
+    <t xml:space="preserve">TRANSMISSION ASSY, PDS</t>
+  </si>
+  <si>
     <t xml:space="preserve">150352-01</t>
   </si>
   <si>
+    <t xml:space="preserve">BEAM, LOWER, FUSELAGE, AFT, RH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150351-01</t>
   </si>
   <si>
+    <t xml:space="preserve">BEAM, LOWER, FUSELAGE, AFT, LH</t>
+  </si>
+  <si>
     <t xml:space="preserve">150350-01</t>
   </si>
   <si>
+    <t xml:space="preserve">PLATE, MAIN, FUSELAGE, AFT</t>
+  </si>
+  <si>
     <t xml:space="preserve">150393-01</t>
   </si>
   <si>
+    <t xml:space="preserve">BUMPER, LANDING GEAR</t>
+  </si>
+  <si>
     <t xml:space="preserve">153336-01</t>
   </si>
   <si>
+    <t xml:space="preserve">FUSELAGE ASSY, FWD</t>
+  </si>
+  <si>
     <t xml:space="preserve">160138-01</t>
   </si>
   <si>
+    <t xml:space="preserve">DPC CONNECTOR BRACE</t>
+  </si>
+  <si>
     <t xml:space="preserve">159978-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABLE HOLDER, ANTENNA, SOB</t>
   </si>
 </sst>
 </file>
@@ -272,7 +494,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -294,6 +516,12 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -303,6 +531,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -348,7 +582,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -372,21 +606,29 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,18 +636,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -477,8 +724,8 @@
   </sheetPr>
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -510,1013 +757,1280 @@
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="C2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>19</v>
+        <v>32</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>21</v>
+        <v>36</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>22</v>
+        <v>38</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>23</v>
+        <v>40</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>24</v>
+        <v>42</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>26</v>
+        <v>46</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>27</v>
+        <v>48</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>28</v>
+        <v>50</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F31" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C32" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F32" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C33" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>30</v>
+        <v>54</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>31</v>
+        <v>56</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C35" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>32</v>
+        <v>58</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="C36" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>33</v>
+        <v>60</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="C37" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>35</v>
+      <c r="A38" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>35</v>
+      <c r="A39" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>35</v>
+      <c r="A40" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>35</v>
+      <c r="A41" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>35</v>
+      <c r="A42" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>35</v>
+      <c r="A43" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>35</v>
+      <c r="A44" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>35</v>
+      <c r="A45" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>35</v>
+      <c r="A46" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>35</v>
+      <c r="A47" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>35</v>
+      <c r="A48" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C49" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>35</v>
+      <c r="A49" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>35</v>
+      <c r="A50" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>35</v>
+      <c r="A51" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C52" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>35</v>
+      <c r="A52" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C53" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>35</v>
+      <c r="A53" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C54" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>35</v>
+      <c r="A54" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C55" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>35</v>
+      <c r="A55" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56" s="5" t="n">
+      <c r="A56" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>35</v>
+      <c r="E56" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C57" s="5" t="e">
+      <c r="A57" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="6" t="e">
         <f aca="false">IF(A57=A56,C56-E56,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E57" s="5" t="s">
-        <v>35</v>
+      <c r="E57" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58" s="5" t="e">
+      <c r="A58" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="6" t="e">
         <f aca="false">IF(A58=A57,C57-E57,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E58" s="5" t="s">
-        <v>35</v>
+      <c r="E58" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C59" s="5" t="e">
+      <c r="A59" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" s="6" t="e">
         <f aca="false">IF(A59=A58,C58-E58,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E59" s="5" t="s">
-        <v>35</v>
+      <c r="E59" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C60" s="5" t="n">
+      <c r="A60" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="E60" s="5" t="s">
-        <v>35</v>
+      <c r="E60" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C61" s="5" t="e">
+      <c r="A61" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" s="6" t="e">
         <f aca="false">IF(A57=A56,C60-E60,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E61" s="5" t="s">
-        <v>35</v>
+      <c r="E61" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C62" s="5" t="n">
+      <c r="A62" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="E62" s="5" t="s">
-        <v>35</v>
+      <c r="E62" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C63" s="5" t="e">
+      <c r="A63" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C63" s="6" t="e">
         <f aca="false">IF(A57=A56,C62-E62,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E63" s="5" t="s">
-        <v>35</v>
+      <c r="E63" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C64" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>35</v>
+      <c r="A64" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C65" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>35</v>
+      <c r="A65" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C65" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C66" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>35</v>
+      <c r="A66" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C67" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>35</v>
+      <c r="A67" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C67" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C68" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>35</v>
+      <c r="A68" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C68" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C69" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>35</v>
+      <c r="A69" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C69" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C70" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>35</v>
+      <c r="A70" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C70" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C71" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>35</v>
+      <c r="A71" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C71" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C72" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>35</v>
+      <c r="A72" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C72" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C73" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>35</v>
+      <c r="A73" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C74" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>35</v>
+      <c r="A74" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C74" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C75" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>35</v>
+      <c r="A75" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C75" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C76" s="5" t="n">
+      <c r="A76" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C76" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="E76" s="5" t="s">
-        <v>35</v>
+      <c r="E76" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C77" s="5" t="e">
+      <c r="A77" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C77" s="6" t="e">
         <f aca="false">IF(A57=A56,C76-E76,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E77" s="5" t="s">
-        <v>35</v>
+      <c r="E77" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C78" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>35</v>
+      <c r="A78" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C78" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C79" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>35</v>
+      <c r="A79" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C79" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C80" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>35</v>
+      <c r="A80" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C80" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C81" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>35</v>
+      <c r="A81" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C82" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>35</v>
+      <c r="A82" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C82" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C83" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>35</v>
+      <c r="A83" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C83" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C84" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>35</v>
+      <c r="A84" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C84" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C85" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>35</v>
+      <c r="A85" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C85" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C86" s="5" t="n">
+      <c r="A86" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C86" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="E86" s="5" t="s">
-        <v>35</v>
+      <c r="E86" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C87" s="5" t="e">
+      <c r="A87" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C87" s="6" t="e">
         <f aca="false">IF(A57=A56,C86-E86,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E87" s="5" t="s">
-        <v>35</v>
+      <c r="E87" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C88" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>35</v>
+      <c r="A88" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C88" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C89" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>35</v>
+      <c r="A89" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C89" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C90" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>35</v>
+      <c r="A90" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C90" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>